<commit_message>
Avance en generwcion de excel a pdf y base64
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/plantilla_acta_v2.xlsx
+++ b/src/main/resources/reports/plantilla_acta_v2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1621B2E-1614-41B0-92FE-D74976A097B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jorge F. Coaquira Ramos</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -334,8 +335,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,185 +632,185 @@
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="17"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="47"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="17"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="47"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,7 +841,13 @@
     <xdr:ext cx="1905000" cy="305612"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1.png"/>
+        <xdr:cNvPr id="3" name="image1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1134,279 +1141,286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="44.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+    </row>
+    <row r="2" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="46" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="50" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
+    <row r="4" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="60"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="19" t="s">
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="21" t="s">
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="30" t="s">
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A13" s="33" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="39" t="s">
+      <c r="I13" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A14" s="40" t="s">
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="57.75" customHeight="1">
-      <c r="A16" s="51" t="s">
+    <row r="16" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-    </row>
-    <row r="18" spans="3:8" ht="49.5" customHeight="1">
-      <c r="C18" s="53" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="18" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55" t="s">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-    </row>
-    <row r="19" spans="3:8" ht="15" customHeight="1">
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58" t="s">
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="59"/>
-      <c r="H19" s="60"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A3:G4"/>
@@ -1419,16 +1433,10 @@
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:H10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="55" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avance de unificacion de creacion, conersion y pendiente de envio a ftp
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/plantilla_acta_v2.xlsx
+++ b/src/main/resources/reports/plantilla_acta_v2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcoaquira\Documents\workspace-spring-tool-suite-4-4.2.2.RELEASE\controlpatrimonial\src\main\resources\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1621B2E-1614-41B0-92FE-D74976A097B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Jorge F. Coaquira Ramos</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,19 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF202429"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>FICHA DE ASIGNACIÓN DE USO Y DEVOLUCIÓN DE BIENES MUEBLES PATRIMONIALES</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <r>
       <rPr>
@@ -101,22 +88,7 @@
     </r>
   </si>
   <si>
-    <t>Fecha:</t>
-  </si>
-  <si>
     <t>${fecha}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color rgb="FF202429"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>DATOS DEL USUARIO</t>
-    </r>
   </si>
   <si>
     <t>NOMBRES Y APELLIDOS</t>
@@ -329,14 +301,46 @@
     <t>_________________________________</t>
   </si>
   <si>
-    <t>____________________________</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF202429"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>FICHA DE ASIGNACIÓN DE USO Y DEVOLUCIÓN DE BIENES MUEBLES PATRIMONIALES</t>
+    </r>
+  </si>
+  <si>
+    <t>FECHA:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202429"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DATOS DEL USUARIO</t>
+    </r>
+  </si>
+  <si>
+    <t>____________________________________</t>
+  </si>
+  <si>
+    <t>TIPO ACTA;</t>
+  </si>
+  <si>
+    <t>${tipo}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,19 +350,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF202429"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="6"/>
       <color rgb="FF202429"/>
       <name val="Arial"/>
@@ -390,13 +381,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF202429"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="6"/>
       <name val="Arial MT"/>
     </font>
@@ -454,6 +438,30 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial MT"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202429"/>
+      <name val="Arial MT"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF202429"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -630,186 +638,174 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="17"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="47"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1141,276 +1137,281 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:9" ht="15.75">
+      <c r="A1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+    </row>
+    <row r="2" spans="1:9" ht="44.25" customHeight="1">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-    </row>
-    <row r="2" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="G5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="54"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="57.75" customHeight="1">
+      <c r="A16" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+    </row>
+    <row r="18" spans="3:8" ht="49.5" customHeight="1">
+      <c r="C18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="3:8" ht="15" customHeight="1">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="46"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-    </row>
-    <row r="18" spans="3:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-    </row>
-    <row r="19" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -1422,7 +1423,6 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A3:G4"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="F18:H18"/>
@@ -1433,9 +1433,10 @@
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:H10"/>
+    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Detallan ajustes de integracion hasta envio de correo, pendiente de ajustes mejores
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/plantilla_acta_v2.xlsx
+++ b/src/main/resources/reports/plantilla_acta_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcoaquira\Documents\workspace-spring-tool-suite-4-4.2.2.RELEASE\controlpatrimonial\src\main\resources\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,16 +405,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF202429"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial mt"/>
-    </font>
-    <font>
       <sz val="5"/>
       <color rgb="FF202429"/>
       <name val="Times New Roman"/>
@@ -462,6 +452,17 @@
       <color rgb="FF202429"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202429"/>
+      <name val="Arial MT"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202429"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -638,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -676,30 +677,51 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="17"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="47"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -709,45 +731,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,23 +797,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="17"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="47"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -1156,73 +1151,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="44.25" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="55" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="55" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1230,101 +1225,101 @@
         <v>5</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="54"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="38"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="48"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="50"/>
       <c r="I10" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1350,78 +1345,71 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="53" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="57.75" customHeight="1">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="18" spans="3:8" ht="49.5" customHeight="1">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="30" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
     </row>
     <row r="19" spans="3:8" ht="15" customHeight="1">
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="A3:G4"/>
     <mergeCell ref="A16:I16"/>
@@ -1434,6 +1422,13 @@
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:H10"/>
     <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>